<commit_message>
Adding small models to test.
The models are a two scenario extensive form with the corresponding submodels present. Experiments will be mainly changing branch bounds and load values.
</commit_message>
<xml_diff>
--- a/list of constraint types.xlsx
+++ b/list of constraint types.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\repos\FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE7C7A75-7280-4A90-BF74-16090BCCE42F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5612C2A8-6945-4D9A-98EB-FFDAF0918207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{25F11CCF-0DEF-4F23-A567-90F21128FEF5}"/>
   </bookViews>
@@ -532,7 +532,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,13 +575,17 @@
       <c r="D2">
         <v>2</v>
       </c>
-      <c r="H2">
+      <c r="G2">
         <f>48+25+C2</f>
         <v>649</v>
       </c>
+      <c r="H2">
+        <f>C2</f>
+        <v>576</v>
+      </c>
       <c r="I2">
-        <f>C2</f>
-        <v>576</v>
+        <f>H4+C2</f>
+        <v>2640</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -601,13 +605,17 @@
       <c r="F3">
         <v>1</v>
       </c>
+      <c r="G3">
+        <f>C3+G2</f>
+        <v>1225</v>
+      </c>
       <c r="H3">
-        <f>C3+H2</f>
-        <v>1225</v>
+        <f>H2+C3</f>
+        <v>1152</v>
       </c>
       <c r="I3">
         <f>I2+C3</f>
-        <v>1152</v>
+        <v>3216</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -627,13 +635,17 @@
       <c r="F4">
         <v>1</v>
       </c>
+      <c r="G4">
+        <f>C4+G3</f>
+        <v>2137</v>
+      </c>
       <c r="H4">
-        <f t="shared" ref="H4:H18" si="0">C4+H3</f>
-        <v>2137</v>
-      </c>
-      <c r="I4">
-        <f>C4+I3</f>
+        <f>C4+H3</f>
         <v>2064</v>
+      </c>
+      <c r="I4" s="1">
+        <f>I3+C4</f>
+        <v>4128</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -650,13 +662,17 @@
       <c r="D5">
         <v>2</v>
       </c>
+      <c r="G5">
+        <f>C5+G4</f>
+        <v>2161</v>
+      </c>
       <c r="H5">
-        <f t="shared" si="0"/>
-        <v>2161</v>
-      </c>
-      <c r="I5">
         <f>48+C5</f>
         <v>72</v>
+      </c>
+      <c r="I5">
+        <f>H11+C5</f>
+        <v>3528</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -673,13 +689,17 @@
       <c r="D6">
         <v>2</v>
       </c>
+      <c r="G6">
+        <f>C6+G5</f>
+        <v>2713</v>
+      </c>
       <c r="H6">
-        <f t="shared" si="0"/>
-        <v>2713</v>
+        <f>C6+H5</f>
+        <v>624</v>
       </c>
       <c r="I6">
-        <f>C6+I5</f>
-        <v>624</v>
+        <f>I5+C6</f>
+        <v>4080</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -696,13 +716,17 @@
       <c r="D7">
         <v>2</v>
       </c>
+      <c r="G7">
+        <f>C7+G6</f>
+        <v>3289</v>
+      </c>
       <c r="H7">
-        <f t="shared" si="0"/>
-        <v>3289</v>
+        <f>C7+H6</f>
+        <v>1200</v>
       </c>
       <c r="I7">
-        <f t="shared" ref="I7:I11" si="1">C7+I6</f>
-        <v>1200</v>
+        <f t="shared" ref="I7:I11" si="0">I6+C7</f>
+        <v>4656</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -719,13 +743,17 @@
       <c r="D8">
         <v>2</v>
       </c>
+      <c r="G8">
+        <f>C8+G7</f>
+        <v>3865</v>
+      </c>
       <c r="H8">
+        <f>C8+H7</f>
+        <v>1776</v>
+      </c>
+      <c r="I8">
         <f t="shared" si="0"/>
-        <v>3865</v>
-      </c>
-      <c r="I8">
-        <f t="shared" si="1"/>
-        <v>1776</v>
+        <v>5232</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -741,13 +769,17 @@
       <c r="D9">
         <v>2</v>
       </c>
+      <c r="G9">
+        <f>C9+G8</f>
+        <v>4441</v>
+      </c>
       <c r="H9">
+        <f>C9+H8</f>
+        <v>2352</v>
+      </c>
+      <c r="I9">
         <f t="shared" si="0"/>
-        <v>4441</v>
-      </c>
-      <c r="I9">
-        <f t="shared" si="1"/>
-        <v>2352</v>
+        <v>5808</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -763,13 +795,17 @@
       <c r="D10">
         <v>2</v>
       </c>
+      <c r="G10">
+        <f>C10+G9</f>
+        <v>5017</v>
+      </c>
       <c r="H10">
+        <f>C10+H9</f>
+        <v>2928</v>
+      </c>
+      <c r="I10">
         <f t="shared" si="0"/>
-        <v>5017</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="1"/>
-        <v>2928</v>
+        <v>6384</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -785,13 +821,17 @@
       <c r="D11">
         <v>2</v>
       </c>
+      <c r="G11">
+        <f>C11+G10</f>
+        <v>5593</v>
+      </c>
       <c r="H11">
+        <f>C11+H10</f>
+        <v>3504</v>
+      </c>
+      <c r="I11" s="1">
         <f t="shared" si="0"/>
-        <v>5593</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="1"/>
-        <v>3504</v>
+        <v>6960</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -810,13 +850,17 @@
       <c r="F12">
         <v>1</v>
       </c>
+      <c r="G12">
+        <f>C12+G11</f>
+        <v>5617</v>
+      </c>
       <c r="H12">
-        <f t="shared" si="0"/>
-        <v>5617</v>
-      </c>
-      <c r="I12">
         <f>25+C12</f>
         <v>49</v>
+      </c>
+      <c r="I12">
+        <f>H16+C12</f>
+        <v>2353</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -833,13 +877,17 @@
       <c r="D13">
         <v>2</v>
       </c>
+      <c r="G13">
+        <f>C13+G12</f>
+        <v>6169</v>
+      </c>
       <c r="H13">
-        <f t="shared" si="0"/>
-        <v>6169</v>
+        <f>H12+C13</f>
+        <v>601</v>
       </c>
       <c r="I13">
         <f>I12+C13</f>
-        <v>601</v>
+        <v>2905</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -858,17 +906,21 @@
       <c r="E14">
         <v>1</v>
       </c>
+      <c r="G14">
+        <f>C14+G13</f>
+        <v>6745</v>
+      </c>
       <c r="H14">
-        <f t="shared" si="0"/>
-        <v>6745</v>
+        <f>H13+C14</f>
+        <v>1177</v>
       </c>
       <c r="I14">
-        <f t="shared" ref="I14:I16" si="2">I13+C14</f>
-        <v>1177</v>
+        <f t="shared" ref="I14:I16" si="1">I13+C14</f>
+        <v>3481</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B15" t="s">
@@ -883,17 +935,21 @@
       <c r="E15">
         <v>1</v>
       </c>
+      <c r="G15">
+        <f>C15+G14</f>
+        <v>7321</v>
+      </c>
       <c r="H15">
-        <f t="shared" si="0"/>
-        <v>7321</v>
+        <f>H14+C15</f>
+        <v>1753</v>
       </c>
       <c r="I15">
-        <f t="shared" si="2"/>
-        <v>1753</v>
+        <f t="shared" si="1"/>
+        <v>4057</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B16" t="s">
@@ -908,17 +964,21 @@
       <c r="E16">
         <v>1</v>
       </c>
+      <c r="G16">
+        <f>C16+G15</f>
+        <v>7897</v>
+      </c>
       <c r="H16">
-        <f t="shared" si="0"/>
-        <v>7897</v>
-      </c>
-      <c r="I16">
-        <f t="shared" si="2"/>
+        <f>H15+C16</f>
         <v>2329</v>
       </c>
+      <c r="I16" s="1">
+        <f t="shared" si="1"/>
+        <v>4633</v>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B17" t="s">
@@ -930,17 +990,21 @@
       <c r="D17">
         <v>2</v>
       </c>
+      <c r="G17">
+        <f>C17+G16</f>
+        <v>8473</v>
+      </c>
       <c r="H17">
-        <f t="shared" si="0"/>
-        <v>8473</v>
+        <f>C17</f>
+        <v>576</v>
       </c>
       <c r="I17">
-        <f>C17</f>
-        <v>576</v>
+        <f>H18+C17</f>
+        <v>2064</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B18" t="s">
@@ -953,13 +1017,17 @@
       <c r="D18">
         <v>2</v>
       </c>
+      <c r="G18">
+        <f>C18+G17</f>
+        <v>9385</v>
+      </c>
       <c r="H18">
-        <f t="shared" si="0"/>
-        <v>9385</v>
-      </c>
-      <c r="I18">
+        <f>H17+C18</f>
+        <v>1488</v>
+      </c>
+      <c r="I18" s="1">
         <f>I17+C18</f>
-        <v>1488</v>
+        <v>2976</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1073,7 +1141,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EABE2865-EBE4-4CDA-B116-0E1B09845A1A}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
@@ -1084,7 +1152,7 @@
     <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -1095,8 +1163,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B2">
@@ -1110,9 +1178,13 @@
         <f>576+48</f>
         <v>624</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="F2">
+        <f>4440+B2</f>
+        <v>5016</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B3">
@@ -1126,9 +1198,13 @@
         <f>E2+B3</f>
         <v>1536</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="F3">
+        <f>F2+B3</f>
+        <v>5928</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B4">
@@ -1142,9 +1218,13 @@
         <f t="shared" ref="E4:E9" si="0">E3+B4</f>
         <v>1560</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="F4">
+        <f t="shared" ref="F4:F9" si="1">F3+B4</f>
+        <v>5952</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B5">
@@ -1158,9 +1238,13 @@
         <f t="shared" si="0"/>
         <v>2136</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>6528</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B6">
@@ -1174,9 +1258,13 @@
         <f t="shared" si="0"/>
         <v>2712</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>7104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B7">
@@ -1190,9 +1278,13 @@
         <f t="shared" si="0"/>
         <v>3288</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>7680</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B8">
@@ -1206,9 +1298,13 @@
         <f t="shared" si="0"/>
         <v>3864</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>8256</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B9">
@@ -1222,8 +1318,12 @@
         <f t="shared" si="0"/>
         <v>4440</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>8832</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>41</v>
       </c>
@@ -1235,7 +1335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>42</v>
       </c>
@@ -1247,7 +1347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12">
         <f>SUM(B2:B11)</f>
         <v>4440</v>

</xml_diff>

<commit_message>
Adding/Checkpointing Step 6 and formalizing extensive form.
</commit_message>
<xml_diff>
--- a/list of constraint types.xlsx
+++ b/list of constraint types.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\repos\FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5612C2A8-6945-4D9A-98EB-FFDAF0918207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B08E311-ADDD-42F6-928B-1DC3114F25D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{25F11CCF-0DEF-4F23-A567-90F21128FEF5}"/>
   </bookViews>
@@ -179,7 +179,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -189,12 +189,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -211,10 +205,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -532,7 +525,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,7 +555,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -589,7 +582,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
@@ -606,7 +599,7 @@
         <v>1</v>
       </c>
       <c r="G3">
-        <f>C3+G2</f>
+        <f t="shared" ref="G3:G18" si="0">C3+G2</f>
         <v>1225</v>
       </c>
       <c r="H3">
@@ -619,7 +612,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
@@ -636,7 +629,7 @@
         <v>1</v>
       </c>
       <c r="G4">
-        <f>C4+G3</f>
+        <f t="shared" si="0"/>
         <v>2137</v>
       </c>
       <c r="H4">
@@ -649,7 +642,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
@@ -663,7 +656,7 @@
         <v>2</v>
       </c>
       <c r="G5">
-        <f>C5+G4</f>
+        <f t="shared" si="0"/>
         <v>2161</v>
       </c>
       <c r="H5">
@@ -676,7 +669,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B6" t="s">
@@ -690,11 +683,11 @@
         <v>2</v>
       </c>
       <c r="G6">
-        <f>C6+G5</f>
+        <f t="shared" si="0"/>
         <v>2713</v>
       </c>
       <c r="H6">
-        <f>C6+H5</f>
+        <f t="shared" ref="H6:H11" si="1">C6+H5</f>
         <v>624</v>
       </c>
       <c r="I6">
@@ -703,7 +696,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B7" t="s">
@@ -717,20 +710,20 @@
         <v>2</v>
       </c>
       <c r="G7">
-        <f>C7+G6</f>
+        <f t="shared" si="0"/>
         <v>3289</v>
       </c>
       <c r="H7">
-        <f>C7+H6</f>
+        <f t="shared" si="1"/>
         <v>1200</v>
       </c>
       <c r="I7">
-        <f t="shared" ref="I7:I11" si="0">I6+C7</f>
+        <f t="shared" ref="I7:I11" si="2">I6+C7</f>
         <v>4656</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B8" t="s">
@@ -744,20 +737,20 @@
         <v>2</v>
       </c>
       <c r="G8">
-        <f>C8+G7</f>
+        <f t="shared" si="0"/>
         <v>3865</v>
       </c>
       <c r="H8">
-        <f>C8+H7</f>
+        <f t="shared" si="1"/>
         <v>1776</v>
       </c>
       <c r="I8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5232</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B9" t="s">
@@ -770,20 +763,20 @@
         <v>2</v>
       </c>
       <c r="G9">
-        <f>C9+G8</f>
+        <f t="shared" si="0"/>
         <v>4441</v>
       </c>
       <c r="H9">
-        <f>C9+H8</f>
+        <f t="shared" si="1"/>
         <v>2352</v>
       </c>
       <c r="I9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5808</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B10" t="s">
@@ -796,20 +789,20 @@
         <v>2</v>
       </c>
       <c r="G10">
-        <f>C10+G9</f>
+        <f t="shared" si="0"/>
         <v>5017</v>
       </c>
       <c r="H10">
-        <f>C10+H9</f>
+        <f t="shared" si="1"/>
         <v>2928</v>
       </c>
       <c r="I10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6384</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B11" t="s">
@@ -822,20 +815,20 @@
         <v>2</v>
       </c>
       <c r="G11">
-        <f>C11+G10</f>
+        <f t="shared" si="0"/>
         <v>5593</v>
       </c>
       <c r="H11">
-        <f>C11+H10</f>
+        <f t="shared" si="1"/>
         <v>3504</v>
       </c>
       <c r="I11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6960</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B12" t="s">
@@ -851,7 +844,7 @@
         <v>1</v>
       </c>
       <c r="G12">
-        <f>C12+G11</f>
+        <f t="shared" si="0"/>
         <v>5617</v>
       </c>
       <c r="H12">
@@ -864,7 +857,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B13" t="s">
@@ -878,7 +871,7 @@
         <v>2</v>
       </c>
       <c r="G13">
-        <f>C13+G12</f>
+        <f t="shared" si="0"/>
         <v>6169</v>
       </c>
       <c r="H13">
@@ -891,7 +884,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B14" t="s">
@@ -907,7 +900,7 @@
         <v>1</v>
       </c>
       <c r="G14">
-        <f>C14+G13</f>
+        <f t="shared" si="0"/>
         <v>6745</v>
       </c>
       <c r="H14">
@@ -915,12 +908,12 @@
         <v>1177</v>
       </c>
       <c r="I14">
-        <f t="shared" ref="I14:I16" si="1">I13+C14</f>
+        <f t="shared" ref="I14:I16" si="3">I13+C14</f>
         <v>3481</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B15" t="s">
@@ -936,7 +929,7 @@
         <v>1</v>
       </c>
       <c r="G15">
-        <f>C15+G14</f>
+        <f t="shared" si="0"/>
         <v>7321</v>
       </c>
       <c r="H15">
@@ -944,12 +937,12 @@
         <v>1753</v>
       </c>
       <c r="I15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4057</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B16" t="s">
@@ -965,7 +958,7 @@
         <v>1</v>
       </c>
       <c r="G16">
-        <f>C16+G15</f>
+        <f t="shared" si="0"/>
         <v>7897</v>
       </c>
       <c r="H16">
@@ -973,12 +966,12 @@
         <v>2329</v>
       </c>
       <c r="I16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4633</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B17" t="s">
@@ -991,7 +984,7 @@
         <v>2</v>
       </c>
       <c r="G17">
-        <f>C17+G16</f>
+        <f t="shared" si="0"/>
         <v>8473</v>
       </c>
       <c r="H17">
@@ -1004,7 +997,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B18" t="s">
@@ -1018,7 +1011,7 @@
         <v>2</v>
       </c>
       <c r="G18">
-        <f>C18+G17</f>
+        <f t="shared" si="0"/>
         <v>9385</v>
       </c>
       <c r="H18">

</xml_diff>

<commit_message>
Adding noint (no interval) models.
</commit_message>
<xml_diff>
--- a/list of constraint types.xlsx
+++ b/list of constraint types.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\repos\FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B08E311-ADDD-42F6-928B-1DC3114F25D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B8FE41C-AAC0-4125-8ECE-150AE7F15E44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{25F11CCF-0DEF-4F23-A567-90F21128FEF5}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="15375" windowHeight="7875" xr2:uid="{25F11CCF-0DEF-4F23-A567-90F21128FEF5}"/>
   </bookViews>
   <sheets>
     <sheet name="constraints" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="50">
   <si>
     <t>Constraint Type</t>
   </si>
@@ -164,6 +164,27 @@
   </si>
   <si>
     <t>ER_expansion</t>
+  </si>
+  <si>
+    <t>by</t>
+  </si>
+  <si>
+    <t>bus</t>
+  </si>
+  <si>
+    <t>branch</t>
+  </si>
+  <si>
+    <t>bus*</t>
+  </si>
+  <si>
+    <t>gen</t>
+  </si>
+  <si>
+    <t>gen*</t>
+  </si>
+  <si>
+    <t>solo</t>
   </si>
 </sst>
 </file>
@@ -205,9 +226,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -522,19 +544,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89213492-71FC-4F0C-B44D-BC806CB808A5}">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -542,588 +564,654 @@
         <v>6</v>
       </c>
       <c r="C1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>16</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2">
         <f>24*24</f>
         <v>576</v>
       </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="G2">
-        <f>48+25+C2</f>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <f>48+25+D2</f>
         <v>649</v>
       </c>
-      <c r="H2">
-        <f>C2</f>
-        <v>576</v>
-      </c>
       <c r="I2">
-        <f>H4+C2</f>
+        <f>D2</f>
+        <v>576</v>
+      </c>
+      <c r="J2">
+        <f>I4+D2</f>
         <v>2640</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3">
         <f>24*24</f>
         <v>576</v>
       </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="F3">
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="G3">
         <v>1</v>
       </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G18" si="0">C3+G2</f>
+      <c r="H3">
+        <f t="shared" ref="H3:H18" si="0">D3+H2</f>
         <v>1225</v>
       </c>
-      <c r="H3">
-        <f>H2+C3</f>
+      <c r="I3">
+        <f>I2+D3</f>
         <v>1152</v>
       </c>
-      <c r="I3">
-        <f>I2+C3</f>
+      <c r="J3">
+        <f>J2+D3</f>
         <v>3216</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4">
         <f>38*24</f>
         <v>912</v>
       </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="F4">
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="G4">
         <v>1</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <f t="shared" si="0"/>
         <v>2137</v>
       </c>
-      <c r="H4">
-        <f>C4+H3</f>
+      <c r="I4">
+        <f>D4+I3</f>
         <v>2064</v>
       </c>
-      <c r="I4" s="1">
-        <f>I3+C4</f>
+      <c r="J4" s="1">
+        <f>J3+D4</f>
         <v>4128</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5">
         <f>1*24</f>
         <v>24</v>
       </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="G5">
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="H5">
         <f t="shared" si="0"/>
         <v>2161</v>
       </c>
-      <c r="H5">
-        <f>48+C5</f>
+      <c r="I5">
+        <f>48+D5</f>
         <v>72</v>
       </c>
-      <c r="I5">
-        <f>H11+C5</f>
+      <c r="J5">
+        <f>I11+D5</f>
         <v>3528</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B6" t="s">
         <v>19</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6">
         <f>24*23</f>
         <v>552</v>
       </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="G6">
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="H6">
         <f t="shared" si="0"/>
         <v>2713</v>
       </c>
-      <c r="H6">
-        <f t="shared" ref="H6:H11" si="1">C6+H5</f>
+      <c r="I6">
+        <f t="shared" ref="I6:I11" si="1">D6+I5</f>
         <v>624</v>
       </c>
-      <c r="I6">
-        <f>I5+C6</f>
+      <c r="J6">
+        <f>J5+D6</f>
         <v>4080</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B7" t="s">
         <v>19</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7">
         <f>24*24</f>
         <v>576</v>
       </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="G7">
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="H7">
         <f t="shared" si="0"/>
         <v>3289</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <f t="shared" si="1"/>
         <v>1200</v>
       </c>
-      <c r="I7">
-        <f t="shared" ref="I7:I11" si="2">I6+C7</f>
+      <c r="J7">
+        <f t="shared" ref="J7:J11" si="2">J6+D7</f>
         <v>4656</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8">
         <f>24*24</f>
         <v>576</v>
       </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="G8">
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="H8">
         <f t="shared" si="0"/>
         <v>3865</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <f t="shared" si="1"/>
         <v>1776</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <f t="shared" si="2"/>
         <v>5232</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B9" t="s">
         <v>19</v>
       </c>
-      <c r="C9">
-        <v>576</v>
+      <c r="C9" t="s">
+        <v>44</v>
       </c>
       <c r="D9">
-        <v>2</v>
-      </c>
-      <c r="G9">
+        <v>576</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="H9">
         <f t="shared" si="0"/>
         <v>4441</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <f t="shared" si="1"/>
         <v>2352</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <f t="shared" si="2"/>
         <v>5808</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B10" t="s">
         <v>19</v>
       </c>
-      <c r="C10">
-        <v>576</v>
+      <c r="C10" t="s">
+        <v>44</v>
       </c>
       <c r="D10">
-        <v>2</v>
-      </c>
-      <c r="G10">
+        <v>576</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="H10">
         <f t="shared" si="0"/>
         <v>5017</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <f t="shared" si="1"/>
         <v>2928</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <f t="shared" si="2"/>
         <v>6384</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
       </c>
-      <c r="C11">
-        <v>576</v>
+      <c r="C11" t="s">
+        <v>44</v>
       </c>
       <c r="D11">
-        <v>2</v>
-      </c>
-      <c r="G11">
+        <v>576</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="H11">
         <f t="shared" si="0"/>
         <v>5593</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <f t="shared" si="1"/>
         <v>3504</v>
       </c>
-      <c r="I11" s="1">
+      <c r="J11" s="1">
         <f t="shared" si="2"/>
         <v>6960</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12">
         <v>24</v>
       </c>
-      <c r="D12">
-        <v>2</v>
-      </c>
-      <c r="F12">
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="G12">
         <v>1</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <f t="shared" si="0"/>
         <v>5617</v>
       </c>
-      <c r="H12">
-        <f>25+C12</f>
+      <c r="I12">
+        <f>25+D12</f>
         <v>49</v>
       </c>
-      <c r="I12">
-        <f>H16+C12</f>
+      <c r="J12">
+        <f>I16+D12</f>
         <v>2353</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B13" t="s">
         <v>8</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13">
         <f>24*23</f>
         <v>552</v>
       </c>
-      <c r="D13">
-        <v>2</v>
-      </c>
-      <c r="G13">
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="H13">
         <f t="shared" si="0"/>
         <v>6169</v>
       </c>
-      <c r="H13">
-        <f>H12+C13</f>
+      <c r="I13">
+        <f>I12+D13</f>
         <v>601</v>
       </c>
-      <c r="I13">
-        <f>I12+C13</f>
+      <c r="J13">
+        <f>J12+D13</f>
         <v>2905</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
       </c>
-      <c r="C14">
-        <v>576</v>
+      <c r="C14" t="s">
+        <v>44</v>
       </c>
       <c r="D14">
-        <v>2</v>
+        <v>576</v>
       </c>
       <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14">
         <v>1</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <f t="shared" si="0"/>
         <v>6745</v>
       </c>
-      <c r="H14">
-        <f>H13+C14</f>
+      <c r="I14">
+        <f>I13+D14</f>
         <v>1177</v>
       </c>
-      <c r="I14">
-        <f t="shared" ref="I14:I16" si="3">I13+C14</f>
+      <c r="J14">
+        <f t="shared" ref="J14:J16" si="3">J13+D14</f>
         <v>3481</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
       </c>
-      <c r="C15">
-        <v>576</v>
+      <c r="C15" t="s">
+        <v>44</v>
       </c>
       <c r="D15">
-        <v>2</v>
+        <v>576</v>
       </c>
       <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15">
         <v>1</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <f t="shared" si="0"/>
         <v>7321</v>
       </c>
-      <c r="H15">
-        <f>H14+C15</f>
+      <c r="I15">
+        <f>I14+D15</f>
         <v>1753</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <f t="shared" si="3"/>
         <v>4057</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B16" t="s">
         <v>8</v>
       </c>
-      <c r="C16">
-        <v>576</v>
+      <c r="C16" t="s">
+        <v>44</v>
       </c>
       <c r="D16">
-        <v>2</v>
+        <v>576</v>
       </c>
       <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
         <v>1</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <f t="shared" si="0"/>
         <v>7897</v>
       </c>
-      <c r="H16">
-        <f>H15+C16</f>
+      <c r="I16">
+        <f>I15+D16</f>
         <v>2329</v>
       </c>
-      <c r="I16" s="1">
+      <c r="J16" s="1">
         <f t="shared" si="3"/>
         <v>4633</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B17" t="s">
         <v>26</v>
       </c>
-      <c r="C17">
-        <v>576</v>
+      <c r="C17" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="D17">
-        <v>2</v>
-      </c>
-      <c r="G17">
+        <v>576</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="H17">
         <f t="shared" si="0"/>
         <v>8473</v>
       </c>
-      <c r="H17">
-        <f>C17</f>
-        <v>576</v>
-      </c>
       <c r="I17">
-        <f>H18+C17</f>
+        <f>D17</f>
+        <v>576</v>
+      </c>
+      <c r="J17">
+        <f>I18+D17</f>
         <v>2064</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B18" t="s">
         <v>26</v>
       </c>
-      <c r="C18">
+      <c r="C18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18">
         <f>38*24</f>
         <v>912</v>
       </c>
-      <c r="D18">
-        <v>2</v>
-      </c>
-      <c r="G18">
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="H18">
         <f t="shared" si="0"/>
         <v>9385</v>
       </c>
-      <c r="H18">
-        <f>H17+C18</f>
+      <c r="I18">
+        <f>I17+D18</f>
         <v>1488</v>
       </c>
-      <c r="I18" s="1">
-        <f>I17+C18</f>
+      <c r="J18" s="1">
+        <f>J17+D18</f>
         <v>2976</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B19" t="s">
         <v>19</v>
       </c>
-      <c r="C19">
+      <c r="C19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19">
         <v>24</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B20" t="s">
         <v>19</v>
       </c>
-      <c r="C20">
+      <c r="C20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20">
         <v>24</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B21" t="s">
         <v>8</v>
       </c>
-      <c r="C21">
+      <c r="C21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21">
         <v>24</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B22" t="s">
         <v>8</v>
       </c>
-      <c r="C22">
-        <v>1</v>
+      <c r="C22" t="s">
+        <v>49</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>30</v>
       </c>
       <c r="B23" t="s">
         <v>2</v>
       </c>
-      <c r="C23">
-        <f>SUM(C2:C4)</f>
+      <c r="D23">
+        <f>SUM(D2:D4)</f>
         <v>2064</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>30</v>
       </c>
       <c r="B24" t="s">
         <v>19</v>
       </c>
-      <c r="C24">
-        <f>SUM(C5:C11)+C19+C20</f>
+      <c r="D24">
+        <f>SUM(D5:D11)+D19+D20</f>
         <v>3504</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>30</v>
       </c>
       <c r="B25" t="s">
         <v>8</v>
       </c>
-      <c r="C25">
-        <f>SUM(C12:C16)+SUM(C21:C22)</f>
+      <c r="D25">
+        <f>SUM(D12:D16)+SUM(D21:D22)</f>
         <v>2329</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>30</v>
       </c>
       <c r="B26" t="s">
         <v>26</v>
       </c>
-      <c r="C26">
-        <f>SUM(C17:C18)</f>
+      <c r="D26">
+        <f>SUM(D17:D18)</f>
         <v>1488</v>
       </c>
     </row>
@@ -1134,216 +1222,256 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EABE2865-EBE4-4CDA-B116-0E1B09845A1A}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>32</v>
       </c>
       <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2">
         <f>24*24</f>
         <v>576</v>
       </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="E2">
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="F2">
         <f>576+48</f>
         <v>624</v>
       </c>
-      <c r="F2">
-        <f>4440+B2</f>
+      <c r="G2">
+        <f>4440+C2</f>
         <v>5016</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3">
         <f>38*24</f>
         <v>912</v>
       </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <f>E2+B3</f>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <f>F2+C3</f>
         <v>1536</v>
       </c>
-      <c r="F3">
-        <f>F2+B3</f>
+      <c r="G3">
+        <f>G2+C3</f>
         <v>5928</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4">
         <f>1*24</f>
         <v>24</v>
       </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <f t="shared" ref="E4:E9" si="0">E3+B4</f>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F9" si="0">F3+C4</f>
         <v>1560</v>
       </c>
-      <c r="F4">
-        <f t="shared" ref="F4:F9" si="1">F3+B4</f>
+      <c r="G4">
+        <f t="shared" ref="G4:G9" si="1">G3+C4</f>
         <v>5952</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5">
         <f>24*24</f>
         <v>576</v>
       </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="E5">
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="F5">
         <f t="shared" si="0"/>
         <v>2136</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <f t="shared" si="1"/>
         <v>6528</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6">
         <f>24*24</f>
         <v>576</v>
       </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="E6">
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="F6">
         <f t="shared" si="0"/>
         <v>2712</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <f t="shared" si="1"/>
         <v>7104</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7">
         <f>24*24</f>
         <v>576</v>
       </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="E7">
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="F7">
         <f t="shared" si="0"/>
         <v>3288</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <f t="shared" si="1"/>
         <v>7680</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8">
         <f>24*24</f>
         <v>576</v>
       </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="E8">
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="F8">
         <f t="shared" si="0"/>
         <v>3864</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <f t="shared" si="1"/>
         <v>8256</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9">
         <f>24*24</f>
         <v>576</v>
       </c>
-      <c r="C9">
-        <v>2</v>
-      </c>
-      <c r="E9">
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="F9">
         <f t="shared" si="0"/>
         <v>4440</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <f t="shared" si="1"/>
         <v>8832</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10">
         <f>24*1</f>
         <v>24</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11">
         <f>24*1</f>
         <v>24</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12">
-        <f>SUM(B2:B11)</f>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <f>SUM(C2:C11)</f>
         <v>4440</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <f>C12-C2-C3</f>
+        <v>2952</v>
       </c>
     </row>
   </sheetData>

</xml_diff>